<commit_message>
analyze static SSD and erasure coding test
</commit_message>
<xml_diff>
--- a/2tier.xlsx
+++ b/2tier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\주우스\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\주우스\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237BF6FA-0E2B-4906-8DFD-04FED884058C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FB908D-CECA-4365-A5E4-601A2D32A774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HW Architecture" sheetId="1" r:id="rId1"/>
@@ -681,14 +681,6 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
-    <t>0.2G</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
-    <t>1.25G</t>
-    <phoneticPr fontId="9" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <rPr>
         <strike/>
@@ -1071,6 +1063,14 @@
   </si>
   <si>
     <t>fds</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>12.5G</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.4G</t>
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
@@ -1663,7 +1663,7 @@
   <dimension ref="A1:AN1062"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="D6" sqref="D6:D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -1708,7 +1708,7 @@
         <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>95</v>
@@ -1824,7 +1824,7 @@
         <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -1870,7 +1870,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -1888,7 +1888,7 @@
         <v>44</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -1901,7 +1901,7 @@
         <v>30</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="2:40" ht="15.75" customHeight="1">
@@ -1912,7 +1912,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="2:40" ht="15.75" customHeight="1">
@@ -1923,7 +1923,7 @@
         <v>33</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="2:40" ht="15.75" customHeight="1">
@@ -1934,7 +1934,7 @@
         <v>35</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>96</v>
@@ -1948,7 +1948,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F10" s="30"/>
     </row>
@@ -1960,7 +1960,7 @@
         <v>38</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F11" s="30"/>
     </row>
@@ -1972,7 +1972,7 @@
         <v>39</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="2:40" ht="15.75" customHeight="1">
@@ -1983,7 +1983,7 @@
         <v>40</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="13"/>
@@ -1997,7 +1997,7 @@
         <v>45</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -2011,13 +2011,13 @@
         <v>46</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
       <c r="H15" s="13"/>
       <c r="L15" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="2:40" ht="15.75" customHeight="1">
@@ -2028,7 +2028,7 @@
         <v>47</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -2042,7 +2042,7 @@
         <v>48</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -2056,7 +2056,7 @@
         <v>49</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
@@ -2070,7 +2070,7 @@
         <v>50</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="15.75" customHeight="1">
@@ -2081,7 +2081,7 @@
         <v>51</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="15.75" customHeight="1">
@@ -2092,7 +2092,7 @@
         <v>52</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="15.75" customHeight="1">
@@ -2103,7 +2103,7 @@
         <v>53</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15.75" customHeight="1">
@@ -2114,7 +2114,7 @@
         <v>54</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="15.75" customHeight="1">
@@ -2125,7 +2125,7 @@
         <v>55</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15.75" customHeight="1">
@@ -2136,7 +2136,7 @@
         <v>56</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15.75" customHeight="1">
@@ -2147,7 +2147,7 @@
         <v>57</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="15.75" customHeight="1">
@@ -2158,7 +2158,7 @@
         <v>58</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="15.75" customHeight="1">
@@ -2169,7 +2169,7 @@
         <v>59</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="15.75" customHeight="1">
@@ -2180,7 +2180,7 @@
         <v>60</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="15.75" customHeight="1">
@@ -2191,7 +2191,7 @@
         <v>61</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="15.75" customHeight="1">
@@ -2202,7 +2202,7 @@
         <v>62</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="15.75" customHeight="1">
@@ -2213,7 +2213,7 @@
         <v>63</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="15.75" customHeight="1">
@@ -2224,7 +2224,7 @@
         <v>64</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="15.75" customHeight="1">
@@ -2235,7 +2235,7 @@
         <v>65</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="15.75" customHeight="1">
@@ -2246,7 +2246,7 @@
         <v>66</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="15.75" customHeight="1">
@@ -2257,7 +2257,7 @@
         <v>67</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="15.75" customHeight="1">
@@ -2268,7 +2268,7 @@
         <v>69</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="15.75" customHeight="1">
@@ -2279,7 +2279,7 @@
         <v>30</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="39" spans="2:4" ht="15.75" customHeight="1">
@@ -2290,7 +2290,7 @@
         <v>31</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="2:4" ht="15.75" customHeight="1">
@@ -2301,7 +2301,7 @@
         <v>32</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="15.75" customHeight="1">
@@ -2312,7 +2312,7 @@
         <v>34</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="15.75" customHeight="1">
@@ -2323,7 +2323,7 @@
         <v>36</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="15.75" customHeight="1">
@@ -2334,7 +2334,7 @@
         <v>38</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="15.75" customHeight="1">
@@ -2345,7 +2345,7 @@
         <v>39</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="15.75" customHeight="1">
@@ -2356,7 +2356,7 @@
         <v>40</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="15.75" customHeight="1">
@@ -2367,7 +2367,7 @@
         <v>45</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="15.75" customHeight="1">
@@ -2378,7 +2378,7 @@
         <v>46</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="15.75" customHeight="1">
@@ -2389,7 +2389,7 @@
         <v>47</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="15.75" customHeight="1">
@@ -2400,7 +2400,7 @@
         <v>48</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="15.75" customHeight="1">
@@ -2411,7 +2411,7 @@
         <v>49</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="15.75" customHeight="1">
@@ -2422,7 +2422,7 @@
         <v>50</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="2:4" ht="15.75" customHeight="1">
@@ -2433,7 +2433,7 @@
         <v>51</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="2:4" ht="15.75" customHeight="1">
@@ -2444,7 +2444,7 @@
         <v>52</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="54" spans="2:4" ht="15.75" customHeight="1">
@@ -2455,7 +2455,7 @@
         <v>53</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="2:4" ht="15.75" customHeight="1">
@@ -2466,7 +2466,7 @@
         <v>54</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="56" spans="2:4" ht="15.75" customHeight="1">
@@ -2477,7 +2477,7 @@
         <v>55</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="15.75" customHeight="1">
@@ -2488,7 +2488,7 @@
         <v>56</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="58" spans="2:4" ht="15.75" customHeight="1">
@@ -2499,7 +2499,7 @@
         <v>57</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59" spans="2:4" ht="15.75" customHeight="1">
@@ -2510,7 +2510,7 @@
         <v>58</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="2:4" ht="15.75" customHeight="1">
@@ -2521,7 +2521,7 @@
         <v>59</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="61" spans="2:4" ht="15.75" customHeight="1">
@@ -2532,7 +2532,7 @@
         <v>60</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="62" spans="2:4" ht="15.75" customHeight="1">
@@ -2543,7 +2543,7 @@
         <v>61</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="63" spans="2:4" ht="15.75" customHeight="1">
@@ -2554,7 +2554,7 @@
         <v>62</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="2:4" ht="15.75" customHeight="1">
@@ -2565,7 +2565,7 @@
         <v>63</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="15.75" customHeight="1">
@@ -2576,7 +2576,7 @@
         <v>64</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="15.75" customHeight="1">
@@ -2587,7 +2587,7 @@
         <v>65</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15.75" customHeight="1">
@@ -2598,7 +2598,7 @@
         <v>66</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="15.75" customHeight="1">
@@ -2609,7 +2609,7 @@
         <v>67</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="15.75" customHeight="1">
@@ -2620,7 +2620,7 @@
         <v>68</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15.75" customHeight="1"/>
@@ -3925,8 +3925,8 @@
   </sheetPr>
   <dimension ref="B1:I1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -3969,11 +3969,11 @@
         <v>233360</v>
       </c>
       <c r="D3" s="4">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E3" s="4">
         <f t="shared" ref="E3:E9" si="0">C3 / (C3+D3)</f>
-        <v>0.9996915589979094</v>
+        <v>0.99989716518698801</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
@@ -3991,11 +3991,11 @@
         <v>41280.840362202769</v>
       </c>
       <c r="D4" s="6">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>0.99825888622475834</v>
+        <v>0.99941895429713457</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
@@ -4013,11 +4013,11 @@
         <v>717739.67029953504</v>
       </c>
       <c r="D5" s="6">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>0.99989969513874033</v>
+        <v>0.99996656281030494</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
@@ -4035,11 +4035,11 @@
         <v>41280.840362202769</v>
       </c>
       <c r="D6" s="4">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>0.99825888622475834</v>
+        <v>0.99941895429713457</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
@@ -4079,11 +4079,11 @@
         <v>700358421.31776893</v>
       </c>
       <c r="D8" s="4">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999989719550675</v>
+        <v>0.99999996573183325</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -4101,11 +4101,11 @@
         <v>700358421.31776893</v>
       </c>
       <c r="D9" s="4">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999989719550675</v>
+        <v>0.99999996573183325</v>
       </c>
       <c r="F9" s="4">
         <v>1</v>
@@ -5116,8 +5116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59A66DAC-66B1-467C-BE75-9DAC5FC70339}">
   <dimension ref="B2:J10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5170,11 +5170,11 @@
       </c>
       <c r="D3" s="17">
         <f>Availability!D3</f>
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E3" s="4">
         <f t="shared" ref="E3:E9" si="0">C3 / (C3+D3)</f>
-        <v>0.9996915589979094</v>
+        <v>0.99989716518698801</v>
       </c>
       <c r="F3" s="4">
         <f>Availability!F3</f>
@@ -5186,14 +5186,14 @@
       </c>
       <c r="H3" s="28">
         <f>1-(1-E3)^2</f>
-        <v>0.99999990486414825</v>
+        <v>0.99999998942500123</v>
       </c>
       <c r="I3" s="28">
         <v>1</v>
       </c>
       <c r="J3" s="28">
         <f>H3^I3</f>
-        <v>0.99999990486414825</v>
+        <v>0.99999998942500123</v>
       </c>
     </row>
     <row r="4" spans="2:10">
@@ -5206,11 +5206,11 @@
       </c>
       <c r="D4" s="17">
         <f>Availability!D4</f>
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>0.99825888622475834</v>
+        <v>0.99941895429713457</v>
       </c>
       <c r="F4" s="4">
         <f>Availability!F4</f>
@@ -5222,14 +5222,14 @@
       </c>
       <c r="H4" s="28">
         <f t="shared" ref="H4:H9" si="1">1-(1-E4)^2</f>
-        <v>0.99999696852282172</v>
+        <v>0.99999966238589122</v>
       </c>
       <c r="I4" s="28">
         <v>2</v>
       </c>
       <c r="J4" s="28">
         <f t="shared" ref="J4:J9" si="2">H4^I4</f>
-        <v>0.9999939370548333</v>
+        <v>0.99999932477189646</v>
       </c>
     </row>
     <row r="5" spans="2:10">
@@ -5242,11 +5242,11 @@
       </c>
       <c r="D5" s="17">
         <f>Availability!D5</f>
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>0.99989969513874033</v>
+        <v>0.99996656281030494</v>
       </c>
       <c r="F5" s="4">
         <f>Availability!F5</f>
@@ -5258,14 +5258,14 @@
       </c>
       <c r="H5" s="28">
         <f t="shared" si="1"/>
-        <v>0.9999999899389348</v>
+        <v>0.99999999888195434</v>
       </c>
       <c r="I5" s="28">
         <v>2</v>
       </c>
       <c r="J5" s="28">
         <f t="shared" si="2"/>
-        <v>0.9999999798778697</v>
+        <v>0.99999999776390869</v>
       </c>
     </row>
     <row r="6" spans="2:10">
@@ -5278,11 +5278,11 @@
       </c>
       <c r="D6" s="17">
         <f>Availability!D6</f>
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>0.99825888622475834</v>
+        <v>0.99941895429713457</v>
       </c>
       <c r="F6" s="4">
         <f>Availability!F6</f>
@@ -5294,14 +5294,14 @@
       </c>
       <c r="H6" s="28">
         <f t="shared" si="1"/>
-        <v>0.99999696852282172</v>
+        <v>0.99999966238589122</v>
       </c>
       <c r="I6" s="28">
         <v>2</v>
       </c>
       <c r="J6" s="28">
         <f t="shared" si="2"/>
-        <v>0.9999939370548333</v>
+        <v>0.99999932477189646</v>
       </c>
     </row>
     <row r="7" spans="2:10">
@@ -5350,11 +5350,11 @@
       </c>
       <c r="D8" s="17">
         <f>Availability!D8</f>
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999989719550675</v>
+        <v>0.99999996573183325</v>
       </c>
       <c r="F8" s="4">
         <f>Availability!F8</f>
@@ -5365,14 +5365,14 @@
       </c>
       <c r="H8" s="28">
         <f>E8</f>
-        <v>0.99999989719550675</v>
+        <v>0.99999996573183325</v>
       </c>
       <c r="I8" s="28">
         <v>1</v>
       </c>
       <c r="J8" s="28">
         <f t="shared" si="2"/>
-        <v>0.99999989719550675</v>
+        <v>0.99999996573183325</v>
       </c>
     </row>
     <row r="9" spans="2:10">
@@ -5385,11 +5385,11 @@
       </c>
       <c r="D9" s="17">
         <f>Availability!D9</f>
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>0.99999989719550675</v>
+        <v>0.99999996573183325</v>
       </c>
       <c r="F9" s="4">
         <f>Availability!F9</f>
@@ -5401,14 +5401,14 @@
       </c>
       <c r="H9" s="28">
         <f t="shared" si="1"/>
-        <v>0.99999999999998945</v>
+        <v>0.99999999999999878</v>
       </c>
       <c r="I9" s="28">
         <v>2</v>
       </c>
       <c r="J9" s="28">
         <f t="shared" si="2"/>
-        <v>0.99999999999997891</v>
+        <v>0.99999999999999756</v>
       </c>
     </row>
     <row r="10" spans="2:10">
@@ -5417,7 +5417,7 @@
       </c>
       <c r="J10">
         <f>PRODUCT(J3:J7)</f>
-        <v>0.99998775121028582</v>
+        <v>0.99999862905353498</v>
       </c>
     </row>
   </sheetData>
@@ -5481,7 +5481,7 @@
         <v>73</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F6" s="20">
         <f>1 /( 1/B6 + 1 / B7 * 4 + 1/B8 + 1/B15)</f>
@@ -5540,7 +5540,7 @@
         <v>75</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F8" s="21">
         <f>E20 * H23/(1-H23)</f>
@@ -5586,10 +5586,10 @@
         <v>9247903</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F10" s="32">
         <f>1 /( 1/B6 * 2 + 1 / B7 * 4 + 1/B8 + 1/B15)</f>
@@ -5675,7 +5675,7 @@
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1">
       <c r="A15" s="33" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B15" s="34">
         <v>43800</v>

</xml_diff>